<commit_message>
Začišťování, obrázky s VOlemortem
</commit_message>
<xml_diff>
--- a/TODO.xlsx
+++ b/TODO.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9372"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9195"/>
   </bookViews>
   <sheets>
     <sheet name="List1" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="151" uniqueCount="150">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="153" uniqueCount="152">
   <si>
     <t>Upravit úvody</t>
   </si>
@@ -500,6 +500,12 @@
   </si>
   <si>
     <t>labelled vs labeled</t>
+  </si>
+  <si>
+    <t>Také si dovedu představit, že se tahle sekce přesune do Introduction (mít pětistránkový introduction není problém).</t>
+  </si>
+  <si>
+    <t>kus výš máte oddělovač tisíců, dal bych ho i sem; každopádně to prosím udělejte konzistentně</t>
   </si>
 </sst>
 </file>
@@ -871,24 +877,24 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B3:P80"/>
+  <dimension ref="B3:P87"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="N33" sqref="N33"/>
+    <sheetView tabSelected="1" topLeftCell="D70" workbookViewId="0">
+      <selection activeCell="H83" sqref="H83"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="70.77734375" customWidth="1"/>
-    <col min="3" max="3" width="11.88671875" style="1" customWidth="1"/>
-    <col min="4" max="4" width="11.33203125" style="1" customWidth="1"/>
-    <col min="5" max="5" width="3.5546875" customWidth="1"/>
-    <col min="6" max="6" width="14.77734375" customWidth="1"/>
-    <col min="8" max="8" width="36.33203125" customWidth="1"/>
-    <col min="14" max="14" width="71.44140625" customWidth="1"/>
+    <col min="2" max="2" width="70.7109375" customWidth="1"/>
+    <col min="3" max="3" width="11.85546875" style="1" customWidth="1"/>
+    <col min="4" max="4" width="11.28515625" style="1" customWidth="1"/>
+    <col min="5" max="5" width="3.5703125" customWidth="1"/>
+    <col min="6" max="6" width="14.7109375" customWidth="1"/>
+    <col min="8" max="8" width="36.28515625" customWidth="1"/>
+    <col min="14" max="14" width="71.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="2:16" x14ac:dyDescent="0.3">
+    <row r="3" spans="2:16" x14ac:dyDescent="0.25">
       <c r="C3" s="1" t="s">
         <v>1</v>
       </c>
@@ -905,7 +911,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="4" spans="2:16" x14ac:dyDescent="0.3">
+    <row r="4" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B4" s="3" t="s">
         <v>4</v>
       </c>
@@ -922,7 +928,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="2:16" x14ac:dyDescent="0.3">
+    <row r="5" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B5" s="4" t="s">
         <v>3</v>
       </c>
@@ -942,7 +948,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="6" spans="2:16" x14ac:dyDescent="0.3">
+    <row r="6" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B6" s="4" t="s">
         <v>5</v>
       </c>
@@ -956,7 +962,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="7" spans="2:16" x14ac:dyDescent="0.3">
+    <row r="7" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B7" s="3" t="s">
         <v>29</v>
       </c>
@@ -970,7 +976,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="8" spans="2:16" x14ac:dyDescent="0.3">
+    <row r="8" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B8" s="3" t="s">
         <v>8</v>
       </c>
@@ -981,7 +987,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="2:16" x14ac:dyDescent="0.3">
+    <row r="9" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B9" s="3" t="s">
         <v>7</v>
       </c>
@@ -992,7 +998,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="10" spans="2:16" x14ac:dyDescent="0.3">
+    <row r="10" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B10" s="3" t="s">
         <v>22</v>
       </c>
@@ -1003,7 +1009,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="11" spans="2:16" x14ac:dyDescent="0.3">
+    <row r="11" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B11" s="3" t="s">
         <v>6</v>
       </c>
@@ -1014,7 +1020,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="12" spans="2:16" x14ac:dyDescent="0.3">
+    <row r="12" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B12" s="3" t="s">
         <v>21</v>
       </c>
@@ -1025,7 +1031,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="13" spans="2:16" x14ac:dyDescent="0.3">
+    <row r="13" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B13" s="3" t="s">
         <v>0</v>
       </c>
@@ -1036,20 +1042,20 @@
         <v>20</v>
       </c>
     </row>
-    <row r="14" spans="2:16" x14ac:dyDescent="0.3">
+    <row r="14" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B14" s="3" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="15" spans="2:16" x14ac:dyDescent="0.3">
+    <row r="15" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B15" s="3" t="s">
         <v>147</v>
       </c>
     </row>
-    <row r="16" spans="2:16" x14ac:dyDescent="0.3">
+    <row r="16" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B16" s="3"/>
     </row>
-    <row r="17" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="17" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B17" s="8" t="s">
         <v>10</v>
       </c>
@@ -1060,7 +1066,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="18" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="18" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B18" s="8" t="s">
         <v>11</v>
       </c>
@@ -1071,7 +1077,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="19" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="19" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B19" s="4" t="s">
         <v>12</v>
       </c>
@@ -1082,7 +1088,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="20" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="20" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B20" s="3" t="s">
         <v>13</v>
       </c>
@@ -1093,7 +1099,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="21" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="21" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B21" s="4" t="s">
         <v>9</v>
       </c>
@@ -1110,7 +1116,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="22" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="22" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B22" s="4" t="s">
         <v>14</v>
       </c>
@@ -1121,7 +1127,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="23" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="23" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B23" s="3" t="s">
         <v>15</v>
       </c>
@@ -1132,13 +1138,13 @@
         <v>10</v>
       </c>
     </row>
-    <row r="24" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="24" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B24" s="3"/>
     </row>
-    <row r="25" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="25" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B25" s="3"/>
     </row>
-    <row r="26" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="26" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B26" s="4" t="s">
         <v>20</v>
       </c>
@@ -1149,7 +1155,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="27" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="27" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B27" s="4" t="s">
         <v>19</v>
       </c>
@@ -1160,7 +1166,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="28" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="28" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B28" s="3" t="s">
         <v>23</v>
       </c>
@@ -1171,7 +1177,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="29" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="29" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B29" s="3" t="s">
         <v>16</v>
       </c>
@@ -1182,7 +1188,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="30" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="30" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B30" s="4" t="s">
         <v>17</v>
       </c>
@@ -1193,7 +1199,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="31" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="31" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B31" s="4" t="s">
         <v>18</v>
       </c>
@@ -1204,18 +1210,18 @@
         <v>20</v>
       </c>
     </row>
-    <row r="33" spans="3:16" x14ac:dyDescent="0.3">
+    <row r="33" spans="3:16" x14ac:dyDescent="0.25">
       <c r="N33" t="s">
         <v>149</v>
       </c>
     </row>
-    <row r="34" spans="3:16" x14ac:dyDescent="0.3">
+    <row r="34" spans="3:16" x14ac:dyDescent="0.25">
       <c r="C34" s="1">
         <f>SUM(C4:C31)</f>
         <v>134</v>
       </c>
     </row>
-    <row r="35" spans="3:16" x14ac:dyDescent="0.3">
+    <row r="35" spans="3:16" x14ac:dyDescent="0.25">
       <c r="C35" s="1">
         <f>C34/15</f>
         <v>8.9333333333333336</v>
@@ -1224,7 +1230,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="36" spans="3:16" x14ac:dyDescent="0.3">
+    <row r="36" spans="3:16" x14ac:dyDescent="0.25">
       <c r="N36" s="3" t="s">
         <v>34</v>
       </c>
@@ -1232,13 +1238,13 @@
         <v>35</v>
       </c>
     </row>
-    <row r="37" spans="3:16" x14ac:dyDescent="0.3">
+    <row r="37" spans="3:16" x14ac:dyDescent="0.25">
       <c r="N37" s="3" t="s">
         <v>36</v>
       </c>
       <c r="O37" s="3"/>
     </row>
-    <row r="38" spans="3:16" x14ac:dyDescent="0.3">
+    <row r="38" spans="3:16" x14ac:dyDescent="0.25">
       <c r="N38" s="3" t="s">
         <v>37</v>
       </c>
@@ -1246,7 +1252,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="39" spans="3:16" x14ac:dyDescent="0.3">
+    <row r="39" spans="3:16" x14ac:dyDescent="0.25">
       <c r="N39" s="3" t="s">
         <v>39</v>
       </c>
@@ -1254,7 +1260,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="40" spans="3:16" x14ac:dyDescent="0.3">
+    <row r="40" spans="3:16" x14ac:dyDescent="0.25">
       <c r="N40" s="3" t="s">
         <v>41</v>
       </c>
@@ -1262,7 +1268,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="41" spans="3:16" x14ac:dyDescent="0.3">
+    <row r="41" spans="3:16" x14ac:dyDescent="0.25">
       <c r="N41" s="3" t="s">
         <v>43</v>
       </c>
@@ -1270,7 +1276,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="42" spans="3:16" x14ac:dyDescent="0.3">
+    <row r="42" spans="3:16" x14ac:dyDescent="0.25">
       <c r="N42" s="3" t="s">
         <v>45</v>
       </c>
@@ -1278,7 +1284,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="43" spans="3:16" x14ac:dyDescent="0.3">
+    <row r="43" spans="3:16" x14ac:dyDescent="0.25">
       <c r="N43" s="3" t="s">
         <v>47</v>
       </c>
@@ -1286,7 +1292,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="44" spans="3:16" x14ac:dyDescent="0.3">
+    <row r="44" spans="3:16" x14ac:dyDescent="0.25">
       <c r="N44" s="3" t="s">
         <v>49</v>
       </c>
@@ -1294,12 +1300,12 @@
         <v>50</v>
       </c>
     </row>
-    <row r="45" spans="3:16" x14ac:dyDescent="0.3">
+    <row r="45" spans="3:16" x14ac:dyDescent="0.25">
       <c r="N45" s="5" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="46" spans="3:16" x14ac:dyDescent="0.3">
+    <row r="46" spans="3:16" x14ac:dyDescent="0.25">
       <c r="N46" s="3" t="s">
         <v>52</v>
       </c>
@@ -1308,7 +1314,7 @@
       </c>
       <c r="P46" s="3"/>
     </row>
-    <row r="47" spans="3:16" x14ac:dyDescent="0.3">
+    <row r="47" spans="3:16" x14ac:dyDescent="0.25">
       <c r="N47" s="3" t="s">
         <v>54</v>
       </c>
@@ -1316,7 +1322,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="48" spans="3:16" x14ac:dyDescent="0.3">
+    <row r="48" spans="3:16" x14ac:dyDescent="0.25">
       <c r="N48" s="3" t="s">
         <v>56</v>
       </c>
@@ -1324,7 +1330,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="49" spans="14:15" x14ac:dyDescent="0.3">
+    <row r="49" spans="14:15" x14ac:dyDescent="0.25">
       <c r="N49" s="3" t="s">
         <v>58</v>
       </c>
@@ -1332,12 +1338,12 @@
         <v>59</v>
       </c>
     </row>
-    <row r="50" spans="14:15" ht="40.200000000000003" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="50" spans="14:15" ht="40.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="N50" s="3" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="51" spans="14:15" x14ac:dyDescent="0.3">
+    <row r="51" spans="14:15" x14ac:dyDescent="0.25">
       <c r="N51" s="3" t="s">
         <v>61</v>
       </c>
@@ -1345,7 +1351,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="52" spans="14:15" x14ac:dyDescent="0.3">
+    <row r="52" spans="14:15" x14ac:dyDescent="0.25">
       <c r="N52" s="3" t="s">
         <v>63</v>
       </c>
@@ -1353,7 +1359,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="53" spans="14:15" x14ac:dyDescent="0.3">
+    <row r="53" spans="14:15" x14ac:dyDescent="0.25">
       <c r="N53" s="3" t="s">
         <v>65</v>
       </c>
@@ -1361,7 +1367,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="54" spans="14:15" x14ac:dyDescent="0.3">
+    <row r="54" spans="14:15" x14ac:dyDescent="0.25">
       <c r="N54" s="3" t="s">
         <v>67</v>
       </c>
@@ -1369,12 +1375,12 @@
         <v>68</v>
       </c>
     </row>
-    <row r="55" spans="14:15" x14ac:dyDescent="0.3">
+    <row r="55" spans="14:15" x14ac:dyDescent="0.25">
       <c r="N55" s="5" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="56" spans="14:15" x14ac:dyDescent="0.3">
+    <row r="56" spans="14:15" x14ac:dyDescent="0.25">
       <c r="N56" s="3" t="s">
         <v>70</v>
       </c>
@@ -1382,7 +1388,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="57" spans="14:15" x14ac:dyDescent="0.3">
+    <row r="57" spans="14:15" x14ac:dyDescent="0.25">
       <c r="N57" s="3" t="s">
         <v>72</v>
       </c>
@@ -1390,7 +1396,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="58" spans="14:15" x14ac:dyDescent="0.3">
+    <row r="58" spans="14:15" x14ac:dyDescent="0.25">
       <c r="N58" s="3" t="s">
         <v>74</v>
       </c>
@@ -1398,12 +1404,12 @@
         <v>75</v>
       </c>
     </row>
-    <row r="59" spans="14:15" x14ac:dyDescent="0.3">
+    <row r="59" spans="14:15" x14ac:dyDescent="0.25">
       <c r="N59" s="5" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="60" spans="14:15" x14ac:dyDescent="0.3">
+    <row r="60" spans="14:15" x14ac:dyDescent="0.25">
       <c r="N60" s="3" t="s">
         <v>77</v>
       </c>
@@ -1411,7 +1417,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="61" spans="14:15" x14ac:dyDescent="0.3">
+    <row r="61" spans="14:15" x14ac:dyDescent="0.25">
       <c r="N61" s="3" t="s">
         <v>79</v>
       </c>
@@ -1419,7 +1425,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="62" spans="14:15" x14ac:dyDescent="0.3">
+    <row r="62" spans="14:15" x14ac:dyDescent="0.25">
       <c r="N62" s="3" t="s">
         <v>81</v>
       </c>
@@ -1427,7 +1433,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="63" spans="14:15" x14ac:dyDescent="0.3">
+    <row r="63" spans="14:15" x14ac:dyDescent="0.25">
       <c r="N63" s="3" t="s">
         <v>83</v>
       </c>
@@ -1435,7 +1441,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="64" spans="14:15" x14ac:dyDescent="0.3">
+    <row r="64" spans="14:15" x14ac:dyDescent="0.25">
       <c r="N64" s="5" t="s">
         <v>85</v>
       </c>
@@ -1443,7 +1449,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="65" spans="14:15" x14ac:dyDescent="0.3">
+    <row r="65" spans="14:15" x14ac:dyDescent="0.25">
       <c r="N65" s="3" t="s">
         <v>87</v>
       </c>
@@ -1451,12 +1457,12 @@
         <v>88</v>
       </c>
     </row>
-    <row r="66" spans="14:15" x14ac:dyDescent="0.3">
+    <row r="66" spans="14:15" x14ac:dyDescent="0.25">
       <c r="N66" s="3" t="s">
         <v>89</v>
       </c>
     </row>
-    <row r="67" spans="14:15" x14ac:dyDescent="0.3">
+    <row r="67" spans="14:15" x14ac:dyDescent="0.25">
       <c r="N67" t="s">
         <v>113</v>
       </c>
@@ -1464,7 +1470,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="68" spans="14:15" x14ac:dyDescent="0.3">
+    <row r="68" spans="14:15" x14ac:dyDescent="0.25">
       <c r="N68" s="3" t="s">
         <v>91</v>
       </c>
@@ -1472,7 +1478,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="69" spans="14:15" x14ac:dyDescent="0.3">
+    <row r="69" spans="14:15" x14ac:dyDescent="0.25">
       <c r="N69" s="3" t="s">
         <v>93</v>
       </c>
@@ -1480,7 +1486,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="70" spans="14:15" x14ac:dyDescent="0.3">
+    <row r="70" spans="14:15" x14ac:dyDescent="0.25">
       <c r="N70" s="3" t="s">
         <v>95</v>
       </c>
@@ -1488,7 +1494,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="71" spans="14:15" x14ac:dyDescent="0.3">
+    <row r="71" spans="14:15" x14ac:dyDescent="0.25">
       <c r="N71" s="3" t="s">
         <v>97</v>
       </c>
@@ -1496,7 +1502,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="72" spans="14:15" x14ac:dyDescent="0.3">
+    <row r="72" spans="14:15" x14ac:dyDescent="0.25">
       <c r="N72" s="5" t="s">
         <v>99</v>
       </c>
@@ -1504,7 +1510,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="73" spans="14:15" x14ac:dyDescent="0.3">
+    <row r="73" spans="14:15" x14ac:dyDescent="0.25">
       <c r="N73" s="3" t="s">
         <v>101</v>
       </c>
@@ -1512,7 +1518,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="74" spans="14:15" x14ac:dyDescent="0.3">
+    <row r="74" spans="14:15" x14ac:dyDescent="0.25">
       <c r="N74" s="3" t="s">
         <v>102</v>
       </c>
@@ -1520,7 +1526,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="75" spans="14:15" x14ac:dyDescent="0.3">
+    <row r="75" spans="14:15" x14ac:dyDescent="0.25">
       <c r="N75" s="3" t="s">
         <v>104</v>
       </c>
@@ -1528,7 +1534,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="76" spans="14:15" x14ac:dyDescent="0.3">
+    <row r="76" spans="14:15" x14ac:dyDescent="0.25">
       <c r="N76" s="3" t="s">
         <v>106</v>
       </c>
@@ -1536,12 +1542,12 @@
         <v>107</v>
       </c>
     </row>
-    <row r="77" spans="14:15" x14ac:dyDescent="0.3">
+    <row r="77" spans="14:15" x14ac:dyDescent="0.25">
       <c r="N77" s="3" t="s">
         <v>108</v>
       </c>
     </row>
-    <row r="78" spans="14:15" x14ac:dyDescent="0.3">
+    <row r="78" spans="14:15" x14ac:dyDescent="0.25">
       <c r="N78" s="3" t="s">
         <v>109</v>
       </c>
@@ -1549,7 +1555,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="79" spans="14:15" x14ac:dyDescent="0.3">
+    <row r="79" spans="14:15" x14ac:dyDescent="0.25">
       <c r="N79" s="5" t="s">
         <v>111</v>
       </c>
@@ -1557,9 +1563,19 @@
         <v>112</v>
       </c>
     </row>
-    <row r="80" spans="14:15" x14ac:dyDescent="0.3">
+    <row r="80" spans="14:15" x14ac:dyDescent="0.25">
       <c r="N80" s="7" t="s">
         <v>148</v>
+      </c>
+    </row>
+    <row r="86" spans="14:14" x14ac:dyDescent="0.25">
+      <c r="N86" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="87" spans="14:14" x14ac:dyDescent="0.25">
+      <c r="N87" t="s">
+        <v>151</v>
       </c>
     </row>
   </sheetData>
@@ -1579,169 +1595,169 @@
       <selection activeCell="K18" sqref="K18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>146</v>
       </c>
     </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>144</v>
       </c>
     </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>123</v>
       </c>
     </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>140</v>
       </c>
     </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>128</v>
       </c>
     </row>
-    <row r="7" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>136</v>
       </c>
     </row>
-    <row r="8" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>121</v>
       </c>
     </row>
-    <row r="9" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>124</v>
       </c>
     </row>
-    <row r="10" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>132</v>
       </c>
     </row>
-    <row r="11" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>125</v>
       </c>
     </row>
-    <row r="12" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>145</v>
       </c>
     </row>
-    <row r="13" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>134</v>
       </c>
     </row>
-    <row r="14" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>122</v>
       </c>
     </row>
-    <row r="15" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>129</v>
       </c>
     </row>
-    <row r="16" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>119</v>
       </c>
     </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>130</v>
       </c>
     </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>142</v>
       </c>
     </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>126</v>
       </c>
     </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>135</v>
       </c>
     </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>143</v>
       </c>
     </row>
-    <row r="22" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>127</v>
       </c>
     </row>
-    <row r="23" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>133</v>
       </c>
     </row>
-    <row r="24" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>139</v>
       </c>
     </row>
-    <row r="25" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>131</v>
       </c>
     </row>
-    <row r="26" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>117</v>
       </c>
     </row>
-    <row r="27" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>118</v>
       </c>
     </row>
-    <row r="28" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>116</v>
       </c>
     </row>
-    <row r="29" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>138</v>
       </c>
     </row>
-    <row r="30" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>141</v>
       </c>
     </row>
-    <row r="31" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>120</v>
       </c>
     </row>
-    <row r="32" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>137</v>
       </c>
     </row>
-    <row r="33" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>114</v>
       </c>
     </row>
-    <row r="34" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>115</v>
       </c>

</xml_diff>